<commit_message>
Add revision history and current template version
</commit_message>
<xml_diff>
--- a/Submission Forms and Templates/Developer Questionnaires/Mobile App AL0 and AL1 iOS Onboarding Questionnaire.xlsx
+++ b/Submission Forms and Templates/Developer Questionnaires/Mobile App AL0 and AL1 iOS Onboarding Questionnaire.xlsx
@@ -1,33 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexduff/Development/ASA-WG/Submission Forms and Templates/Developer Questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326842D8-7160-B845-9A1D-9A8B8CC317F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C022AA-F97E-7E42-B7F6-7F166EAC11C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="21660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="21660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" r:id="rId1"/>
-    <sheet name="Storage" sheetId="2" r:id="rId2"/>
-    <sheet name="Crypto" sheetId="3" r:id="rId3"/>
-    <sheet name="Network" sheetId="4" r:id="rId4"/>
-    <sheet name="Platform" sheetId="5" r:id="rId5"/>
-    <sheet name="Resilience" sheetId="6" r:id="rId6"/>
-    <sheet name="Privacy" sheetId="7" r:id="rId7"/>
-    <sheet name="Files" sheetId="8" r:id="rId8"/>
+    <sheet name="Revision History" sheetId="9" r:id="rId2"/>
+    <sheet name="Storage" sheetId="2" r:id="rId3"/>
+    <sheet name="Crypto" sheetId="3" r:id="rId4"/>
+    <sheet name="Network" sheetId="4" r:id="rId5"/>
+    <sheet name="Platform" sheetId="5" r:id="rId6"/>
+    <sheet name="Resilience" sheetId="6" r:id="rId7"/>
+    <sheet name="Privacy" sheetId="7" r:id="rId8"/>
+    <sheet name="Files" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="97">
   <si>
     <t>ID</t>
   </si>
@@ -391,12 +392,45 @@
   <si>
     <t>v1.0</t>
   </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Alex Duff</t>
+  </si>
+  <si>
+    <t>Add template version and revision history</t>
+  </si>
+  <si>
+    <t>Default profile versions to 1.0. No test guide version.</t>
+  </si>
+  <si>
+    <t>Kevin Baker</t>
+  </si>
+  <si>
+    <t>Add profile and test guide version row.</t>
+  </si>
+  <si>
+    <t>Brad Ree</t>
+  </si>
+  <si>
+    <t>Initial revision</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -442,6 +476,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -481,10 +530,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -511,9 +561,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="15" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{8733A448-537B-FF4B-92EC-6AB5A39F06B1}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -731,7 +785,7 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -861,6 +915,96 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F59CCF45-57FA-E246-ABF6-5201F2F39AC6}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="3" width="10.83203125" style="11"/>
+    <col min="4" max="4" width="42.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" s="11">
+        <v>4</v>
+      </c>
+      <c r="B2" s="12">
+        <v>46049</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="11">
+        <v>3</v>
+      </c>
+      <c r="B3" s="12">
+        <v>46038</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12">
+        <v>46036</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="11">
+        <v>1</v>
+      </c>
+      <c r="B5" s="12">
+        <v>45999</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3915,7 +4059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -6960,7 +7104,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -7015,7 +7159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -10094,7 +10238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -13129,7 +13273,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -16171,7 +16315,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>